<commit_message>
first attempt of linear interpolation of xyz positions onto LEDs - currently didn't seem to work but requires further testing
</commit_message>
<xml_diff>
--- a/segment_start_end_indexes.xlsx
+++ b/segment_start_end_indexes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>FOG-LAW</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>8bit</t>
+  </si>
+  <si>
+    <t>16bit</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>rounded x 100:</t>
   </si>
 </sst>
 </file>
@@ -120,8 +138,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -155,6 +191,15 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -164,6 +209,15 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,15 +547,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L18" sqref="L18:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -529,8 +586,29 @@
       <c r="I1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -564,8 +642,32 @@
         <f>VLOOKUP($C2,led_positions!$A$2:$D$339,4)</f>
         <v>13.2248</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="L2">
+        <f>ROUND(D2*100,0)</f>
+        <v>-4836</v>
+      </c>
+      <c r="M2">
+        <f>ROUND(E2*100,0)</f>
+        <v>-3825</v>
+      </c>
+      <c r="N2">
+        <f>ROUND(F2*100,0)</f>
+        <v>2878</v>
+      </c>
+      <c r="O2">
+        <f>ROUND(G2*100,0)</f>
+        <v>-4544</v>
+      </c>
+      <c r="P2">
+        <f>ROUND(H2*100,0)</f>
+        <v>-1312</v>
+      </c>
+      <c r="Q2">
+        <f>ROUND(I2*100,0)</f>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -599,8 +701,32 @@
         <f>VLOOKUP($C3,led_positions!$A$2:$D$339,4)</f>
         <v>21.974299999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="L3">
+        <f>ROUND(D3*100,0)</f>
+        <v>-2883</v>
+      </c>
+      <c r="M3">
+        <f>ROUND(E3*100,0)</f>
+        <v>919</v>
+      </c>
+      <c r="N3">
+        <f>ROUND(F3*100,0)</f>
+        <v>2151</v>
+      </c>
+      <c r="O3">
+        <f>ROUND(G3*100,0)</f>
+        <v>-864</v>
+      </c>
+      <c r="P3">
+        <f>ROUND(H3*100,0)</f>
+        <v>-2561</v>
+      </c>
+      <c r="Q3">
+        <f>ROUND(I3*100,0)</f>
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -634,8 +760,32 @@
         <f>VLOOKUP($C4,led_positions!$A$2:$D$339,4)</f>
         <v>7.2907000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4">
+        <f>ROUND(D4*100,0)</f>
+        <v>-30</v>
+      </c>
+      <c r="M4">
+        <f>ROUND(E4*100,0)</f>
+        <v>-57</v>
+      </c>
+      <c r="N4">
+        <f>ROUND(F4*100,0)</f>
+        <v>9</v>
+      </c>
+      <c r="O4">
+        <f>ROUND(G4*100,0)</f>
+        <v>-2486</v>
+      </c>
+      <c r="P4">
+        <f>ROUND(H4*100,0)</f>
+        <v>-4705</v>
+      </c>
+      <c r="Q4">
+        <f>ROUND(I4*100,0)</f>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -669,8 +819,32 @@
         <f>VLOOKUP($C5,led_positions!$A$2:$D$339,4)</f>
         <v>0.451847575</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="L5">
+        <f>ROUND(D5*100,0)</f>
+        <v>-848</v>
+      </c>
+      <c r="M5">
+        <f>ROUND(E5*100,0)</f>
+        <v>-2513</v>
+      </c>
+      <c r="N5">
+        <f>ROUND(F5*100,0)</f>
+        <v>2156</v>
+      </c>
+      <c r="O5">
+        <f>ROUND(G5*100,0)</f>
+        <v>-18</v>
+      </c>
+      <c r="P5">
+        <f>ROUND(H5*100,0)</f>
+        <v>-53</v>
+      </c>
+      <c r="Q5">
+        <f>ROUND(I5*100,0)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -704,8 +878,32 @@
         <f>VLOOKUP($C6,led_positions!$A$2:$D$339,4)</f>
         <v>29.122599999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="L6">
+        <f>ROUND(D6*100,0)</f>
+        <v>-2532</v>
+      </c>
+      <c r="M6">
+        <f>ROUND(E6*100,0)</f>
+        <v>-4688</v>
+      </c>
+      <c r="N6">
+        <f>ROUND(F6*100,0)</f>
+        <v>772</v>
+      </c>
+      <c r="O6">
+        <f>ROUND(G6*100,0)</f>
+        <v>-4842</v>
+      </c>
+      <c r="P6">
+        <f>ROUND(H6*100,0)</f>
+        <v>-3880</v>
+      </c>
+      <c r="Q6">
+        <f>ROUND(I6*100,0)</f>
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -738,6 +936,421 @@
       <c r="I7">
         <f>VLOOKUP($C7,led_positions!$A$2:$D$339,4)</f>
         <v>21.5014</v>
+      </c>
+      <c r="L7">
+        <f>ROUND(D7*100,0)</f>
+        <v>-4507</v>
+      </c>
+      <c r="M7">
+        <f>ROUND(E7*100,0)</f>
+        <v>-1261</v>
+      </c>
+      <c r="N7">
+        <f>ROUND(F7*100,0)</f>
+        <v>1341</v>
+      </c>
+      <c r="O7">
+        <f>ROUND(G7*100,0)</f>
+        <v>-2916</v>
+      </c>
+      <c r="P7">
+        <f>ROUND(H7*100,0)</f>
+        <v>975</v>
+      </c>
+      <c r="Q7">
+        <f>ROUND(I7*100,0)</f>
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <f>MAX(D2:I7)</f>
+        <v>29.122599999999998</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <f>MIN(D2:I7)</f>
+        <v>-48.424599999999998</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
+        <f>ROUND(255*(D2-$D$10)/$D$11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" ref="M10:Q10" si="0">ROUND(255*(E2-$D$10)/$D$11,0)</f>
+        <v>33</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="0"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <f>D9-D10</f>
+        <v>77.547200000000004</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1">
+        <f t="shared" ref="L11:L15" si="1">ROUND(255*(D3-$D$10)/$D$11,0)</f>
+        <v>64</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" ref="M11:M15" si="2">ROUND(255*(E3-$D$10)/$D$11,0)</f>
+        <v>189</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" ref="N11:N15" si="3">ROUND(255*(F3-$D$10)/$D$11,0)</f>
+        <v>230</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O15" si="4">ROUND(255*(G3-$D$10)/$D$11,0)</f>
+        <v>131</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" ref="P11:P15" si="5">ROUND(255*(H3-$D$10)/$D$11,0)</f>
+        <v>75</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" ref="Q11:Q15" si="6">ROUND(255*(I3-$D$10)/$D$11,0)</f>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
+        <f t="shared" si="1"/>
+        <v>158</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="6"/>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="4"/>
+        <v>159</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="5"/>
+        <v>158</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="6"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="3"/>
+        <v>185</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="5"/>
+        <v>191</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="6"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="11:17">
+      <c r="K17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="11:17">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1">
+        <f>ROUND(65535*(D2-$D$10)/$D$11,0)</f>
+        <v>55</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" ref="M18:Q18" si="7">ROUND(65535*(E2-$D$10)/$D$11,0)</f>
+        <v>8601</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="7"/>
+        <v>65245</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="7"/>
+        <v>2523</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="7"/>
+        <v>29835</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="7"/>
+        <v>52100</v>
+      </c>
+    </row>
+    <row r="19" spans="11:17">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1">
+        <f t="shared" ref="L19:L23" si="8">ROUND(65535*(D3-$D$10)/$D$11,0)</f>
+        <v>16556</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" ref="M19:M23" si="9">ROUND(65535*(E3-$D$10)/$D$11,0)</f>
+        <v>48686</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" ref="N19:N23" si="10">ROUND(65535*(F3-$D$10)/$D$11,0)</f>
+        <v>59101</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" ref="O19:O23" si="11">ROUND(65535*(G3-$D$10)/$D$11,0)</f>
+        <v>33619</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" ref="P19:P23" si="12">ROUND(65535*(H3-$D$10)/$D$11,0)</f>
+        <v>19278</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" ref="Q19:Q23" si="13">ROUND(65535*(I3-$D$10)/$D$11,0)</f>
+        <v>59494</v>
+      </c>
+    </row>
+    <row r="20" spans="11:17">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1">
+        <f t="shared" si="8"/>
+        <v>40667</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="9"/>
+        <v>40438</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="10"/>
+        <v>40999</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="11"/>
+        <v>19918</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="12"/>
+        <v>1164</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="13"/>
+        <v>47085</v>
+      </c>
+    </row>
+    <row r="21" spans="11:17">
+      <c r="K21" s="1"/>
+      <c r="L21" s="1">
+        <f t="shared" si="8"/>
+        <v>33756</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="9"/>
+        <v>19686</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="10"/>
+        <v>59144</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="11"/>
+        <v>40773</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="12"/>
+        <v>40478</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="13"/>
+        <v>41305</v>
+      </c>
+    </row>
+    <row r="22" spans="11:17">
+      <c r="K22" s="1"/>
+      <c r="L22" s="1">
+        <f t="shared" si="8"/>
+        <v>19523</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="9"/>
+        <v>1302</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="10"/>
+        <v>47450</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="12"/>
+        <v>8132</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="13"/>
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="23" spans="11:17">
+      <c r="K23" s="1"/>
+      <c r="L23" s="1">
+        <f t="shared" si="8"/>
+        <v>2831</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="9"/>
+        <v>30269</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="10"/>
+        <v>52257</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="11"/>
+        <v>16278</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="12"/>
+        <v>49166</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="13"/>
+        <v>59094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>